<commit_message>
setting up ADC polling. Deal with the interruption.
</commit_message>
<xml_diff>
--- a/Расчет частоты.xlsx
+++ b/Расчет частоты.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio\STM32_Project\studyMCU_103\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2D7CE6-D739-4A34-8160-1D3E2878D558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03BF1CB-D861-4A3D-90F0-12A43048525F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11220" yWindow="3310" windowWidth="20510" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>Тактовая частота МК</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Расчет частоты для ADC IN8 temperature: TIM2</t>
+  </si>
+  <si>
+    <t>mс</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -178,25 +181,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -488,7 +494,7 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,11 +505,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="1">
         <v>64</v>
       </c>
@@ -513,10 +519,10 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -553,23 +559,23 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
@@ -599,11 +605,11 @@
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="1">
         <v>63</v>
       </c>
@@ -613,11 +619,11 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="6">
         <v>2399</v>
       </c>
@@ -625,11 +631,11 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
       <c r="T5" s="9">
         <v>2399</v>
       </c>
@@ -638,11 +644,11 @@
       <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="1">
         <v>49</v>
       </c>
@@ -652,11 +658,11 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
       <c r="L6" s="6">
         <v>9999</v>
       </c>
@@ -664,11 +670,11 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
       <c r="T6" s="9">
         <v>5999</v>
       </c>
@@ -677,11 +683,11 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="1">
         <f>1/(D1/(D5+1)/(D6+1))</f>
         <v>50</v>
@@ -692,11 +698,11 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
       <c r="L7" s="6">
         <f>D1*1000000/(L5+1)/(L6+1)</f>
         <v>2.666666666666667</v>
@@ -712,11 +718,11 @@
         <v>11</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="12" t="s">
+      <c r="Q7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
       <c r="T7" s="9">
         <f>D1*1000000/(T5+1)/(T6+1)</f>
         <v>4.4444444444444446</v>
@@ -741,11 +747,11 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
       <c r="L8" s="6">
         <f>1/L7*10^6</f>
         <v>374999.99999999994</v>
@@ -761,11 +767,11 @@
         <v>13</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="Q8" s="12" t="s">
+      <c r="Q8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
       <c r="T8" s="9">
         <f>1/T7*10^6</f>
         <v>224999.99999999997</v>
@@ -801,22 +807,22 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -843,23 +849,23 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="6">
-        <v>1919</v>
+        <v>639</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="6">
         <v>0</v>
       </c>
@@ -870,13 +876,13 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="6">
-        <v>6665</v>
+        <v>19999</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="1"/>
@@ -885,11 +891,11 @@
         <v>254</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="6">
         <v>29</v>
       </c>
@@ -900,14 +906,14 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="6">
         <f>D1*1000000/(D12+1)/(D13+1)</f>
-        <v>5.0005000500050008</v>
+        <v>5</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>5</v>
@@ -915,11 +921,11 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="6">
         <f>D1*1000000/(L12+1)/(L13+1)</f>
         <v>2133333.3333333335</v>
@@ -938,14 +944,14 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="6">
         <f>1/D14*10^6</f>
-        <v>199980</v>
+        <v>200000</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>4</v>
@@ -953,11 +959,11 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="6">
         <f>1/L14*10^6</f>
         <v>0.46874999999999994</v>
@@ -971,11 +977,18 @@
       <c r="Q15" s="8"/>
     </row>
     <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.4">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="11">
+        <f>1/D14*10^3</f>
+        <v>200</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1">
@@ -993,10 +1006,10 @@
       <c r="Q16" s="8"/>
     </row>
     <row r="17" spans="1:17" ht="17" x14ac:dyDescent="0.4">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1031,9 +1044,9 @@
       <c r="Q18" s="8"/>
     </row>
     <row r="19" spans="1:17" ht="17" x14ac:dyDescent="0.4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="1"/>
@@ -1050,9 +1063,9 @@
       <c r="Q19" s="8"/>
     </row>
     <row r="20" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
@@ -1069,9 +1082,9 @@
       <c r="Q20" s="8"/>
     </row>
     <row r="21" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
@@ -1088,9 +1101,9 @@
       <c r="Q21" s="8"/>
     </row>
     <row r="22" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
@@ -1164,18 +1177,12 @@
       <c r="Q25" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A3:E3"/>
+  <mergeCells count="32">
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A19:C19"/>
@@ -1191,11 +1198,18 @@
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="I12:K12"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>